<commit_message>
main para ejecutar etl
</commit_message>
<xml_diff>
--- a/app/data/maestros.xlsx
+++ b/app/data/maestros.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SergioRetuertoGutier\Documents\Projects\attsf\attsf-ordenes-de-trabajo\app\data\maestros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SergioRetuertoGutier\Documents\Projects\attsf\attsf-ordenes-de-trabajo\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F07A7B-93DD-44FF-BA5C-36768ED365B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06564B64-D512-4A6F-B17A-1B80D0A26E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="camion" sheetId="1" r:id="rId1"/>
@@ -4066,7 +4066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -12700,16 +12700,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E359"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12738,10 +12738,10 @@
         <v>423</v>
       </c>
       <c r="C2" s="3">
-        <v>277321</v>
+        <v>27.732080980572398</v>
       </c>
       <c r="D2" s="3">
-        <v>-801831</v>
+        <v>-8.0183106077851996</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>456</v>
@@ -12756,10 +12756,10 @@
         <v>387</v>
       </c>
       <c r="C3" s="3">
-        <v>276147</v>
+        <v>27.614697279679699</v>
       </c>
       <c r="D3" s="3">
-        <v>-786977</v>
+        <v>-7869766227805630</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>457</v>
@@ -12774,10 +12774,10 @@
         <v>426</v>
       </c>
       <c r="C4" s="3">
-        <v>275064</v>
+        <v>27.506362076684599</v>
       </c>
       <c r="D4" s="3">
-        <v>-800828</v>
+        <v>-8008280197426500</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>458</v>
@@ -12792,7 +12792,7 @@
         <v>425</v>
       </c>
       <c r="C5" s="3">
-        <v>268257</v>
+        <v>26.825700000000001</v>
       </c>
       <c r="D5" s="3">
         <v>-686468</v>
@@ -12810,7 +12810,7 @@
         <v>424</v>
       </c>
       <c r="C6" s="3">
-        <v>274951</v>
+        <v>27.495100000000001</v>
       </c>
       <c r="D6" s="3">
         <v>-782654</v>

</xml_diff>

<commit_message>
actualizar maestro de wilayas
</commit_message>
<xml_diff>
--- a/app/data/maestros.xlsx
+++ b/app/data/maestros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SergioRetuertoGutier\Documents\Projects\attsf\attsf-ordenes-de-trabajo\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06564B64-D512-4A6F-B17A-1B80D0A26E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B239981-A33A-4085-BF88-9E5BB28B00B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12701,7 +12701,7 @@
   <dimension ref="A1:E359"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12759,7 +12759,7 @@
         <v>27.614697279679699</v>
       </c>
       <c r="D3" s="3">
-        <v>-7869766227805630</v>
+        <v>-7.8697662278056297</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>457</v>
@@ -12777,7 +12777,7 @@
         <v>27.506362076684599</v>
       </c>
       <c r="D4" s="3">
-        <v>-8008280197426500</v>
+        <v>-8.0082801974264992</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>458</v>
@@ -12795,7 +12795,7 @@
         <v>26.825700000000001</v>
       </c>
       <c r="D5" s="3">
-        <v>-686468</v>
+        <v>-6.8646799999999999</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>459</v>
@@ -12813,7 +12813,7 @@
         <v>27.495100000000001</v>
       </c>
       <c r="D6" s="3">
-        <v>-782654</v>
+        <v>-7.8265399999999996</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>460</v>
@@ -12828,10 +12828,10 @@
         <v>461</v>
       </c>
       <c r="C7" s="3">
-        <v>27482</v>
+        <v>27.481999999999999</v>
       </c>
       <c r="D7" s="3">
-        <v>-809825</v>
+        <v>-8.0982500000000002</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>462</v>

</xml_diff>